<commit_message>
Send max hp to Client. Initial Parameter Class made
</commit_message>
<xml_diff>
--- a/Engine/data/datasheet/boss_parameter.xlsx
+++ b/Engine/data/datasheet/boss_parameter.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\datasheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14F7B038-28F7-4FCF-8AE0-0C41E8735AB9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0118243F-8116-454D-AB1D-AFF6E4A97648}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9285"/>
+    <workbookView xWindow="14730" yWindow="1020" windowWidth="12420" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="boss_parameter" sheetId="1" r:id="rId1"/>
@@ -20,16 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
-  <si>
-    <t>BOSS_HP</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>BOSS_DAMAGE</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="14">
   <si>
     <t>BOSS_SPEED</t>
   </si>
@@ -71,24 +62,12 @@
   </si>
   <si>
     <t>BOSS_COLLIDER_SIZE_Z</t>
-  </si>
-  <si>
-    <t>BOSS_PHASE3_HP</t>
-  </si>
-  <si>
-    <t>보스가 페이즈3로 넘어가는 체력 %</t>
-  </si>
-  <si>
-    <t>BOSS_PHASE2_HP</t>
-  </si>
-  <si>
-    <t>보스가 페이즈2로 넘어가는 체력 %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1033,11 +1012,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1045,197 +1024,147 @@
     <col min="1" max="1" width="24.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>8</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>9</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>3</v>
       </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>3</v>
       </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="C12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
       <c r="B13">
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>0.3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17">
-        <v>0.6</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>